<commit_message>
Make Habib plots nicer.
</commit_message>
<xml_diff>
--- a/data/Habib2013.xlsx
+++ b/data/Habib2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="3980" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15240" yWindow="7800" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FFT Titan" sheetId="1" r:id="rId1"/>
@@ -243,11 +243,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076178872"/>
-        <c:axId val="1801723560"/>
+        <c:axId val="-2129338216"/>
+        <c:axId val="-2129331304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076178872"/>
+        <c:axId val="-2129338216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,12 +276,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1801723560"/>
+        <c:crossAx val="-2129331304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1801723560"/>
+        <c:axId val="-2129331304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -311,7 +311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076178872"/>
+        <c:crossAx val="-2129338216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -422,11 +422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900033304"/>
-        <c:axId val="1801618456"/>
+        <c:axId val="-2129267368"/>
+        <c:axId val="-2129261912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900033304"/>
+        <c:axId val="-2129267368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -455,12 +455,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1801618456"/>
+        <c:crossAx val="-2129261912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1801618456"/>
+        <c:axId val="-2129261912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900033304"/>
+        <c:crossAx val="-2129267368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -698,11 +698,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900953160"/>
-        <c:axId val="1900843032"/>
+        <c:axId val="-2129225096"/>
+        <c:axId val="-2129219576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900953160"/>
+        <c:axId val="-2129225096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -733,13 +733,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900843032"/>
+        <c:crossAx val="-2129219576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1900843032"/>
+        <c:axId val="-2129219576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,7 +779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900953160"/>
+        <c:crossAx val="-2129225096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -941,11 +941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900540376"/>
-        <c:axId val="1900545848"/>
+        <c:axId val="-2129190920"/>
+        <c:axId val="-2129185432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900540376"/>
+        <c:axId val="-2129190920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,12 +974,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900545848"/>
+        <c:crossAx val="-2129185432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1900545848"/>
+        <c:axId val="-2129185432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1020,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900540376"/>
+        <c:crossAx val="-2129190920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1323,11 +1323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900635368"/>
-        <c:axId val="1900832824"/>
+        <c:axId val="-2129136456"/>
+        <c:axId val="-2129130936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900635368"/>
+        <c:axId val="-2129136456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -1358,13 +1358,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900832824"/>
+        <c:crossAx val="-2129130936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1900832824"/>
+        <c:axId val="-2129130936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,10 +1372,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -1404,7 +1404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900635368"/>
+        <c:crossAx val="-2129136456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,38 +1472,14 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>('Full Titan'!$B$2:$B$10,'Full Titan'!$B$18)</c:f>
+              <c:f>('Full Titan'!$B$2,'Full Titan'!$B$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>265.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4069.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>16384.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1511,38 +1487,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Full Titan'!$M$2:$M$10,'Full Titan'!$M$18)</c:f>
+              <c:f>('Full Titan'!$M$2,'Full Titan'!$M$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>50.67144311634715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.33572155817357</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.66786077908679</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.118815772540033</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.166965194771697</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.583482597385848</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.791741298692924</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.398497463682258</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.197935324673231</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0.0989676623366155</c:v>
                 </c:pt>
               </c:numCache>
@@ -1712,11 +1664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900421576"/>
-        <c:axId val="1801770088"/>
+        <c:axId val="-2129094792"/>
+        <c:axId val="-2129089272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900421576"/>
+        <c:axId val="-2129094792"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1748,13 +1700,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1801770088"/>
+        <c:crossAx val="-2129089272"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1801770088"/>
+        <c:axId val="-2129089272"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1764,10 +1716,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -1796,7 +1748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900421576"/>
+        <c:crossAx val="-2129094792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1864,38 +1816,14 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>('Full Titan'!$B$2:$B$10,'Full Titan'!$B$18)</c:f>
+              <c:f>('Full Titan'!$B$2,'Full Titan'!$B$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>265.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4069.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>16384.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1903,38 +1831,14 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Full Titan'!$L$2:$L$10,'Full Titan'!$L$18)</c:f>
+              <c:f>('Full Titan'!$L$2,'Full Titan'!$L$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.97349816484186E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.94699632968373E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.89399265936746E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.63430316775967E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.15759706374698E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.31519412749396E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.26303882549879E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.50942626023173E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.05215530199517E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>1.01043106039903E10</c:v>
                 </c:pt>
               </c:numCache>
@@ -2104,11 +2008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900065864"/>
-        <c:axId val="1900071336"/>
+        <c:axId val="-2129055224"/>
+        <c:axId val="-2129049704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900065864"/>
+        <c:axId val="-2129055224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2139,13 +2043,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900071336"/>
+        <c:crossAx val="-2129049704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1900071336"/>
+        <c:axId val="-2129049704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0E10"/>
@@ -2154,10 +2058,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -2174,7 +2078,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Rate (particles/second)</a:t>
+                  <a:t>Rate (Particles/Second)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2186,7 +2090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900065864"/>
+        <c:crossAx val="-2129055224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -2401,11 +2305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1900412680"/>
-        <c:axId val="1900709496"/>
+        <c:axId val="-2129018024"/>
+        <c:axId val="-2129012504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1900412680"/>
+        <c:axId val="-2129018024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2436,13 +2340,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900709496"/>
+        <c:crossAx val="-2129012504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1900709496"/>
+        <c:axId val="-2129012504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2451,10 +2355,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -2483,7 +2387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1900412680"/>
+        <c:crossAx val="-2129018024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2692,11 +2596,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1914361576"/>
-        <c:axId val="1914357688"/>
+        <c:axId val="-2128982024"/>
+        <c:axId val="-2128976504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1914361576"/>
+        <c:axId val="-2128982024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2727,13 +2631,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1914357688"/>
+        <c:crossAx val="-2128976504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1914357688"/>
+        <c:axId val="-2128976504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2741,10 +2645,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -2773,7 +2677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1914361576"/>
+        <c:crossAx val="-2128982024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3827,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
A mistake in the numbers alerted by Tim.
</commit_message>
<xml_diff>
--- a/data/Habib2013.xlsx
+++ b/data/Habib2013.xlsx
@@ -156,7 +156,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -243,11 +242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129338216"/>
-        <c:axId val="-2129331304"/>
+        <c:axId val="-2087835800"/>
+        <c:axId val="-2087806664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129338216"/>
+        <c:axId val="-2087835800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,19 +268,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129331304"/>
+        <c:crossAx val="-2087806664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129331304"/>
+        <c:axId val="-2087806664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,14 +302,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129338216"/>
+        <c:crossAx val="-2087835800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -358,7 +355,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -422,11 +418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129267368"/>
-        <c:axId val="-2129261912"/>
+        <c:axId val="-2147326056"/>
+        <c:axId val="-2147420776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129267368"/>
+        <c:axId val="-2147326056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,19 +444,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129261912"/>
+        <c:crossAx val="-2147420776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129261912"/>
+        <c:axId val="-2147420776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,14 +478,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129267368"/>
+        <c:crossAx val="-2147326056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -698,11 +692,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129225096"/>
-        <c:axId val="-2129219576"/>
+        <c:axId val="-2087792232"/>
+        <c:axId val="-2087787992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129225096"/>
+        <c:axId val="-2087792232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -726,20 +720,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129219576"/>
+        <c:crossAx val="-2087787992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129219576"/>
+        <c:axId val="-2087787992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,21 +765,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129225096"/>
+        <c:crossAx val="-2087792232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -941,11 +932,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129190920"/>
-        <c:axId val="-2129185432"/>
+        <c:axId val="-2087745864"/>
+        <c:axId val="-2087740376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129190920"/>
+        <c:axId val="-2087745864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,19 +958,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129185432"/>
+        <c:crossAx val="-2087740376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129185432"/>
+        <c:axId val="-2087740376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1013,21 +1003,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129190920"/>
+        <c:crossAx val="-2087745864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1097,7 +1085,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -1109,7 +1097,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -1136,7 +1124,7 @@
                   <c:v>12.66786077908679</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.118815772540033</c:v>
+                  <c:v>6.333930389543394</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.166965194771697</c:v>
@@ -1148,7 +1136,7 @@
                   <c:v>0.791741298692924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.398497463682258</c:v>
+                  <c:v>0.395870649346462</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.197935324673231</c:v>
@@ -1257,7 +1245,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -1269,7 +1257,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -1323,11 +1311,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129136456"/>
-        <c:axId val="-2129130936"/>
+        <c:axId val="-2087462216"/>
+        <c:axId val="-2087456696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129136456"/>
+        <c:axId val="-2087462216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -1358,13 +1346,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129130936"/>
+        <c:crossAx val="-2087456696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129130936"/>
+        <c:axId val="-2087456696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129136456"/>
+        <c:crossAx val="-2087462216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1598,7 +1586,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -1610,7 +1598,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -1664,11 +1652,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129094792"/>
-        <c:axId val="-2129089272"/>
+        <c:axId val="-2087420776"/>
+        <c:axId val="-2087415256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129094792"/>
+        <c:axId val="-2087420776"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1700,13 +1688,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129089272"/>
+        <c:crossAx val="-2087415256"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129089272"/>
+        <c:axId val="-2087415256"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1748,7 +1736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129094792"/>
+        <c:crossAx val="-2087420776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1942,7 +1930,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -1954,7 +1942,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -2008,11 +1996,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129055224"/>
-        <c:axId val="-2129049704"/>
+        <c:axId val="-2087381240"/>
+        <c:axId val="-2087375720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129055224"/>
+        <c:axId val="-2087381240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2043,13 +2031,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129049704"/>
+        <c:crossAx val="-2087375720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129049704"/>
+        <c:axId val="-2087375720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0E10"/>
@@ -2090,7 +2078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129055224"/>
+        <c:crossAx val="-2087381240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -2239,7 +2227,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -2251,7 +2239,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -2275,7 +2263,7 @@
                   <c:v>0.655366062561889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.607120480924921</c:v>
+                  <c:v>0.628464560332437</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.619244400883785</c:v>
@@ -2287,7 +2275,7 @@
                   <c:v>0.359050726013794</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.209389791670659</c:v>
+                  <c:v>0.208009536696268</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.158085090167875</c:v>
@@ -2305,11 +2293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129018024"/>
-        <c:axId val="-2129012504"/>
+        <c:axId val="-2087344360"/>
+        <c:axId val="-2087338840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2129018024"/>
+        <c:axId val="-2087344360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2340,13 +2328,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129012504"/>
+        <c:crossAx val="-2087338840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129012504"/>
+        <c:axId val="-2087338840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2387,7 +2375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129018024"/>
+        <c:crossAx val="-2087344360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2530,7 +2518,7 @@
                   <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>512.0</c:v>
@@ -2542,7 +2530,7 @@
                   <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4069.0</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8192.0</c:v>
@@ -2596,11 +2584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128982024"/>
-        <c:axId val="-2128976504"/>
+        <c:axId val="-2087308232"/>
+        <c:axId val="-2087302712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128982024"/>
+        <c:axId val="-2087308232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16384.0"/>
@@ -2631,13 +2619,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128976504"/>
+        <c:crossAx val="-2087302712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4096.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128976504"/>
+        <c:axId val="-2087302712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +2665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128982024"/>
+        <c:crossAx val="-2087308232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3731,9 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3945,7 +3931,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C5">
         <v>28.097999999999999</v>
@@ -3972,23 +3958,23 @@
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>2867.7298541374521</v>
+        <v>2770.3352553176896</v>
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>2.6707815510569625E-6</v>
+        <v>2.5800757625304997E-6</v>
       </c>
       <c r="K5">
         <f t="shared" si="6"/>
-        <v>0.60712048092492077</v>
+        <v>0.62846456033243747</v>
       </c>
       <c r="L5">
         <f t="shared" si="7"/>
-        <v>163430316.77596685</v>
+        <v>157879853.18734911</v>
       </c>
       <c r="M5">
         <f t="shared" si="8"/>
-        <v>6.1188157725400334</v>
+        <v>6.3339303895433936</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -4149,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>4069</v>
+        <v>4096</v>
       </c>
       <c r="C9">
         <v>7.8259999999999996</v>
@@ -4176,23 +4162,23 @@
       </c>
       <c r="I9">
         <f t="shared" si="4"/>
-        <v>8314.9112204339126</v>
+        <v>8370.0851213805126</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>7.7438645255136421E-6</v>
+        <v>7.795249224994809E-6</v>
       </c>
       <c r="K9">
         <f t="shared" si="6"/>
-        <v>0.2093897916706591</v>
+        <v>0.20800953669626754</v>
       </c>
       <c r="L9">
         <f t="shared" si="7"/>
-        <v>2509426260.2317324</v>
+        <v>2526077650.9975858</v>
       </c>
       <c r="M9">
         <f t="shared" si="8"/>
-        <v>0.3984974636822583</v>
+        <v>0.3958706493464621</v>
       </c>
     </row>
     <row r="10" spans="1:13">

</xml_diff>